<commit_message>
Ajout des images de Benji
</commit_message>
<xml_diff>
--- a/MS - Miscellanous, Finish & Assembly/Cost/Cost_MS_cor_CME_et_PAT.xlsx
+++ b/MS - Miscellanous, Finish & Assembly/Cost/Cost_MS_cor_CME_et_PAT.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0D4FA8-FB3F-4FFC-B2A6-784EA68B017B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634405E2-3118-48E9-A5FB-D0B7F0A8C099}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="3870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="3870" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="22" r:id="rId1"/>
@@ -146,7 +146,7 @@
     <definedName name="MS_A0500_q">'MS A0500'!$N$3</definedName>
     <definedName name="MS_A0500_t">'MS A0500'!$I$34</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2630,21 +2630,131 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>125910</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41DA9A48-E738-4711-86C3-19D9631DFBCA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12496800" y="4838700"/>
+          <a:ext cx="3390900" cy="3681910"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>39708</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152950</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E09BE619-E38B-4987-905A-BB5CB59B5516}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5838825" y="39708"/>
+          <a:ext cx="2105025" cy="1637242"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>259081</xdr:colOff>
+      <xdr:colOff>281941</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7455247" cy="5660627"/>
+    <xdr:ext cx="6899222" cy="5294862"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Image 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56A7A5F2-26A6-48E0-8965-346F6E0C0070}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F3DE9D1-B59E-469F-AF08-656AB6EB4850}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2660,8 +2770,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="259081" y="297180"/>
-          <a:ext cx="7455247" cy="5660627"/>
+          <a:off x="281941" y="304800"/>
+          <a:ext cx="6899222" cy="5294862"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2673,7 +2783,357 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142586</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FCCF5A7-5C0A-4FA9-8E2F-428E35D79D75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5810250" y="28576"/>
+          <a:ext cx="2124075" cy="1638010"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6813663" cy="5180571"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{518D3F26-A49C-462F-9942-920E3A3EB114}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="259080" y="312420"/>
+          <a:ext cx="6813663" cy="5180571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>139574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC7BDE74-0879-4AA4-88CD-5F4404748AA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5895975" y="47625"/>
+          <a:ext cx="2114550" cy="1615949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7165203" cy="5498698"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0144C6A-7130-4817-A9A6-47B4FE6E0783}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="213360" y="198120"/>
+          <a:ext cx="7165203" cy="5498698"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1304925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>164278</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{370A45F7-473A-4711-8FCC-E684D66AD1BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="66676"/>
+          <a:ext cx="1876425" cy="1621602"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7006892" cy="5355827"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7030F8-FF1F-4051-8F0B-22477A27ABCA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="320040" y="266700"/>
+          <a:ext cx="7006892" cy="5355827"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>552290</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>121664</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1993404" cy="2372056"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{247EA8A0-80C2-4F9C-A0B6-21BCBF486EC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6648290" y="2979164"/>
+          <a:ext cx="1993404" cy="2372056"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -2723,7 +3183,62 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>965200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>52498</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552426</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{673B0EA2-D373-4410-8AB4-D825970A470B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="52498"/>
+          <a:ext cx="1581126" cy="1598502"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2779,7 +3294,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -2829,7 +3344,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2885,7 +3400,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing23.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -2935,7 +3450,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing24.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -2986,7 +3501,107 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>259081</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7455247" cy="5660627"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56A7A5F2-26A6-48E0-8965-346F6E0C0070}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="259081" y="297180"/>
+          <a:ext cx="7455247" cy="5660627"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>826283</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>90523</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>797099</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A916615-A90C-40C6-8951-2670C8EC1966}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5936165" y="90523"/>
+          <a:ext cx="1976669" cy="1444683"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -3031,7 +3646,62 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>172101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{730F2782-0212-41B7-98B9-2DB6F2D270C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7629526" y="2324100"/>
+          <a:ext cx="2076449" cy="1467501"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -3076,7 +3746,62 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1123950</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>132312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E8E2C80-ABED-4990-BFF7-5EAA4587E42B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5915025" y="28575"/>
+          <a:ext cx="2047875" cy="1627737"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -3110,236 +3835,6 @@
         <a:xfrm>
           <a:off x="205740" y="304800"/>
           <a:ext cx="6818156" cy="5241522"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>281941</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="6899222" cy="5294862"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F3DE9D1-B59E-469F-AF08-656AB6EB4850}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="281941" y="304800"/>
-          <a:ext cx="6899222" cy="5294862"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="6813663" cy="5180571"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{518D3F26-A49C-462F-9942-920E3A3EB114}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="259080" y="312420"/>
-          <a:ext cx="6813663" cy="5180571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7165203" cy="5498698"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0144C6A-7130-4817-A9A6-47B4FE6E0783}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="213360" y="198120"/>
-          <a:ext cx="7165203" cy="5498698"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7006892" cy="5355827"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7030F8-FF1F-4051-8F0B-22477A27ABCA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="320040" y="266700"/>
-          <a:ext cx="7006892" cy="5355827"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>552290</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>121664</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1993404" cy="2372056"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{247EA8A0-80C2-4F9C-A0B6-21BCBF486EC4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6648290" y="2979164"/>
-          <a:ext cx="1993404" cy="2372056"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3756,12 +4251,12 @@
   </sheetPr>
   <dimension ref="A1:FG171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H10" sqref="H10"/>
       <selection pane="topRight" activeCell="H10" sqref="H10"/>
       <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7907,6 +8402,7 @@
     <hyperlink ref="G2" location="MS_0100_005_BOM" display="Back to BOM" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7949,7 +8445,7 @@
   </sheetPr>
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -8464,6 +8960,7 @@
     <hyperlink ref="G2" location="MS_0100_006_BOM" display="Back to BOM" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9023,6 +9520,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9578,6 +10076,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9588,8 +10087,8 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10267,8 +10766,8 @@
   </sheetPr>
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12402,6 +12901,7 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="70" max="16383" man="1"/>
   </rowBreaks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -18341,7 +18841,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18891,6 +19391,7 @@
     <brk id="19" max="16383" man="1"/>
     <brk id="53" max="16383" man="1"/>
   </rowBreaks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -18974,7 +19475,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19484,6 +19985,7 @@
     <hyperlink ref="G2" location="MS_0100_002_BOM" display="Back to BOM" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -19528,7 +20030,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20069,6 +20571,7 @@
     <hyperlink ref="G2" location="MS_0100_003_BOM" display="Back to BOM" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -20627,5 +21130,6 @@
     <hyperlink ref="G2" location="MS_0100_004_BOM" display="Back to BOM" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>